<commit_message>
Cambios COSEDE, LDAP, SSO, VENTANAS ASISTENCIAS, MANTENIMIENTOS
</commit_message>
<xml_diff>
--- a/public/Excels/tabla_base_BIENES_TECNOLOGICOS.xlsx
+++ b/public/Excels/tabla_base_BIENES_TECNOLOGICOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leito\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBC0B81-BDA0-45FC-93FA-0FF564DC98C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C9AD1B-5297-4ED5-9A0C-8CAB7A0B8978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D4F9E16-9883-4C0F-8F7B-90AD2D520C20}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{2D4F9E16-9883-4C0F-8F7B-90AD2D520C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2FCB9C-79E6-4DCD-98C5-82F0614D4175}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +698,7 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>730854</v>
       </c>
       <c r="B2" s="2">

</xml_diff>